<commit_message>
Actualizacion avance FunctionsApachePoi.java NumericValues.java
</commit_message>
<xml_diff>
--- a/documents/procesedDocuments/TablaDinamica.xlsx
+++ b/documents/procesedDocuments/TablaDinamica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mairon.martinez\Desktop\BUMaironMartinez\BACKUP\MiBanco\_081-RQ-SIARIndicadoresDeCalidadDelPortafolio\documents\procesedDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D31F74-C2CF-49D2-B352-6FF606978DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A59357A-35D7-424D-9ED8-D5C1C5725C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="8">
   <si>
     <t>TipoProducto</t>
   </si>
@@ -52,18 +49,6 @@
   </si>
   <si>
     <t>cocina</t>
-  </si>
-  <si>
-    <t>Suma de Cantidad</t>
-  </si>
-  <si>
-    <t>Etiquetas de columna</t>
-  </si>
-  <si>
-    <t>Etiquetas de fila</t>
-  </si>
-  <si>
-    <t>Total general</t>
   </si>
 </sst>
 </file>
@@ -99,13 +84,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -121,221 +101,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Mairon Santiago Martinez Rojas" refreshedDate="45180.748164930556" createdVersion="3" refreshedVersion="7" minRefreshableVersion="3" recordCount="18" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:C19" sheet="Hoja1"/>
-  </cacheSource>
-  <cacheFields count="3">
-    <cacheField name="TipoProducto" numFmtId="0">
-      <sharedItems count="5">
-        <s v="bebida"/>
-        <s v="legumbre"/>
-        <s v="lacteo"/>
-        <s v="aseo"/>
-        <s v="cocina"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="producto" numFmtId="0">
-      <sharedItems count="5">
-        <s v="bebida"/>
-        <s v="legumbre"/>
-        <s v="lacteo"/>
-        <s v="aseo"/>
-        <s v="cocina"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="cantidad" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="18"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="18">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="5"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <n v="6"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <n v="7"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="8"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="9"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="4"/>
-    <n v="10"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <n v="11"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="12"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="13"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="4"/>
-    <n v="14"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <n v="15"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="16"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="17"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="18"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" multipleFieldFilters="0">
-  <location ref="E13:K20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de Cantidad" fld="2" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,16 +377,9 @@
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -643,7 +401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -654,7 +412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -665,7 +423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -676,7 +434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -687,7 +445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -698,7 +456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -709,7 +467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -720,7 +478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -731,7 +489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -742,7 +500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -753,7 +511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -763,14 +521,8 @@
       <c r="C13">
         <v>12</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -780,29 +532,8 @@
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -812,21 +543,8 @@
       <c r="C15">
         <v>14</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="3">
-        <v>75</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -836,21 +554,8 @@
       <c r="C16">
         <v>15</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3">
-        <v>33</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -860,21 +565,8 @@
       <c r="C17">
         <v>16</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3">
-        <v>17</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -884,21 +576,8 @@
       <c r="C18">
         <v>17</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3">
-        <v>22</v>
-      </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -907,42 +586,6 @@
       </c>
       <c r="C19">
         <v>18</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3">
-        <v>24</v>
-      </c>
-      <c r="K19" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="3">
-        <v>75</v>
-      </c>
-      <c r="G20" s="3">
-        <v>33</v>
-      </c>
-      <c r="H20" s="3">
-        <v>17</v>
-      </c>
-      <c r="I20" s="3">
-        <v>22</v>
-      </c>
-      <c r="J20" s="3">
-        <v>24</v>
-      </c>
-      <c r="K20" s="3">
-        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>